<commit_message>
Refactor dependencies for week 3
</commit_message>
<xml_diff>
--- a/final/tests/4.3.1_test_set.xlsx
+++ b/final/tests/4.3.1_test_set.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagefleming/university_of_london/current_courses/agile_software_projects/cm2020/final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagefleming/university_of_london/current_courses/agile_software_projects/cm2020/final/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD187763-ECE5-CF4C-9CC7-71D771D71EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE00689-FC50-EE4D-AB75-9A8B475B266B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.3.1 Jan-19th" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="77">
   <si>
     <t>Objective and Priority</t>
   </si>
@@ -101,15 +101,6 @@
   </si>
   <si>
     <t>4.3.1.2</t>
-  </si>
-  <si>
-    <t>Continue to test 4.3.1.2.1</t>
-  </si>
-  <si>
-    <t>Continue to test 4.3.1.1.2</t>
-  </si>
-  <si>
-    <t>Continue to test 4.3.2.1.1</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -193,36 +184,15 @@
     <t>FINISHED</t>
   </si>
   <si>
-    <t>Continue to test 4.3.1.3.1</t>
-  </si>
-  <si>
-    <t>4.3.1.2.1 Dropdown.Whitelist.Toggle</t>
-  </si>
-  <si>
-    <t>4.3.1.1.1 Dropdown.SettingsButtons</t>
-  </si>
-  <si>
-    <t>4.3.1.2.2 Dropdown.Whitelist.QuickDelete</t>
-  </si>
-  <si>
     <t>Test Result</t>
   </si>
   <si>
-    <t>4.3.1.3.1 Dropdown.TimeTracker.Display</t>
-  </si>
-  <si>
-    <t>4.3.1.3.2 Dropdown.TimeTracker.StatsButton</t>
-  </si>
-  <si>
     <t>Startup: Open browser, click on StudySync extension dropdown</t>
   </si>
   <si>
     <t>Check if the settings button redirects to settings page</t>
   </si>
   <si>
-    <t>4.3.1.1.1 Dropdown.SettingsButton</t>
-  </si>
-  <si>
     <t>Settings button redirects user to settings pages.</t>
   </si>
   <si>
@@ -238,12 +208,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>StudySync shall delete a whitelist item if it’s corresponding trashcan button is clicked on by the user.</t>
-  </si>
-  <si>
-    <t>10 minutes</t>
-  </si>
-  <si>
     <t>Click on the trashcan icon next to whitelist item.</t>
   </si>
   <si>
@@ -256,9 +220,6 @@
     <t>No list options appear.</t>
   </si>
   <si>
-    <t>Test that StudySync displays the current course and task being tracked along with the total time spent on the current task.</t>
-  </si>
-  <si>
     <t>Displays placeholder data.</t>
   </si>
   <si>
@@ -272,6 +233,33 @@
   </si>
   <si>
     <t>Does not update.</t>
+  </si>
+  <si>
+    <t>4.3.1.2.2.1 Dropdown.Whitelist.Toggle</t>
+  </si>
+  <si>
+    <t>4.3.1.2.2.2 Dropdown.Whitelist.QuickDelete</t>
+  </si>
+  <si>
+    <t>4.3.1.2.1.1 Dropdown.SettingsButtons</t>
+  </si>
+  <si>
+    <t>4.3.1.2.3.1 Dropdown.TimeTracker.Display</t>
+  </si>
+  <si>
+    <t>4.3.1.2.3.2 Dropdown.TimeTracker.StatsButton</t>
+  </si>
+  <si>
+    <t>Continue to test 4.3.1.2.2.1</t>
+  </si>
+  <si>
+    <t>Continue to test 4.3.1.2.2.2</t>
+  </si>
+  <si>
+    <t>Continue to test 4.3.1.2.3.1</t>
+  </si>
+  <si>
+    <t>Continue to test 4.3.1.2.3.2</t>
   </si>
 </sst>
 </file>
@@ -439,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -462,6 +450,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -469,7 +532,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -480,60 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -543,26 +552,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,110 +943,118 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="30" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="30" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="30"/>
-    <col min="8" max="8" width="29" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="30" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="30"/>
-    <col min="14" max="14" width="26" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" style="30" customWidth="1"/>
-    <col min="16" max="16" width="20.5" style="30" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" style="30" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" style="30"/>
-    <col min="20" max="20" width="16.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36" style="30" customWidth="1"/>
-    <col min="22" max="22" width="28.6640625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="29.6640625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.6640625" style="30"/>
+    <col min="1" max="1" width="3.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="16"/>
+    <col min="8" max="8" width="29" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="16"/>
+    <col min="14" max="14" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="16" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="16" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="16"/>
+    <col min="20" max="20" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" style="16" customWidth="1"/>
+    <col min="22" max="22" width="28.6640625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="25" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="H4" s="25" t="s">
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="N4" s="25" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="25"/>
-    </row>
-    <row r="5" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="P4" s="15"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G5" s="25"/>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="M5" s="25"/>
       <c r="N5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1068,88 +1067,93 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:18" ht="28" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="25"/>
       <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="13"/>
+      <c r="O6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="H7" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="N7" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="34"/>
-    </row>
-    <row r="8" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="25"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="35"/>
-    </row>
-    <row r="9" spans="2:18" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:18" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1165,6 +1169,7 @@
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="G9" s="25"/>
       <c r="H9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1180,6 +1185,7 @@
       <c r="L9" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="M9" s="25"/>
       <c r="N9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1192,26 +1198,27 @@
       <c r="Q9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="R9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="56" x14ac:dyDescent="0.15">
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>65</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="25"/>
       <c r="H10" s="2">
         <v>1</v>
       </c>
@@ -1222,33 +1229,35 @@
         <v>12</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" s="20" t="s">
-        <v>68</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="25"/>
       <c r="N10" s="2">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R10" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+      <c r="R10" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="56" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="2">
         <v>2</v>
       </c>
@@ -1259,146 +1268,155 @@
         <v>14</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>65</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="25"/>
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="H12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="N12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
-    </row>
-    <row r="13" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-    </row>
-    <row r="14" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="26" t="s">
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="N12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="H14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="26" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J14" s="15"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G15" s="25"/>
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="30" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="15" t="s">
+    <row r="16" spans="2:18" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="G16" s="25"/>
       <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="28" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="H17" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="8" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1414,6 +1432,7 @@
       <c r="F19" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="G19" s="25"/>
       <c r="H19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1430,238 +1449,230 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:12" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>68</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="25"/>
       <c r="H20" s="2">
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" s="30" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L20" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>65</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="25"/>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="24"/>
-    </row>
-    <row r="22" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="2:12" ht="28" x14ac:dyDescent="0.15">
       <c r="B22" s="2">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="19" t="s">
         <v>65</v>
       </c>
+      <c r="F22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="25"/>
       <c r="H22" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="2:12" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12" ht="56" x14ac:dyDescent="0.15">
       <c r="B23" s="2">
         <v>4</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B24" s="2">
         <v>5</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-    </row>
-    <row r="25" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-    </row>
-    <row r="26" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B26" s="2">
         <v>7</v>
       </c>
-      <c r="C26" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B27" s="2">
         <v>8</v>
       </c>
-      <c r="C27" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-    </row>
-    <row r="28" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B28" s="2"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="1"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="H29" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B29" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="C6:E6"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="I15:K15"/>
@@ -1669,6 +1680,22 @@
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1684,107 +1711,111 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" style="30" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="30"/>
-    <col min="8" max="8" width="29" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="30" customWidth="1"/>
-    <col min="12" max="12" width="16.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="30"/>
-    <col min="14" max="14" width="26" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" style="30" customWidth="1"/>
-    <col min="16" max="16" width="27.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.6640625" style="30"/>
-    <col min="20" max="20" width="16.5" style="30" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36" style="30" customWidth="1"/>
-    <col min="22" max="22" width="28.6640625" style="30" customWidth="1"/>
-    <col min="23" max="23" width="29.6640625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="17.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.6640625" style="30"/>
+    <col min="1" max="1" width="3.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="16"/>
+    <col min="8" max="8" width="29" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="16"/>
+    <col min="14" max="14" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="16" customWidth="1"/>
+    <col min="16" max="16" width="27.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="16"/>
+    <col min="20" max="20" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" style="16" customWidth="1"/>
+    <col min="22" max="22" width="28.6640625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.6640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-    </row>
-    <row r="2" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="25" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="25"/>
-      <c r="H4" s="25" t="s">
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="N4" s="25" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="N4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="O4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="25"/>
-    </row>
-    <row r="5" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G5" s="25"/>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1800,88 +1831,91 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:18" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:18" ht="28" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G6" s="25"/>
       <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="13"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="H7" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="N7" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="34"/>
-    </row>
-    <row r="8" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="8" t="s">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="N7" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="35"/>
-    </row>
-    <row r="9" spans="2:18" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="2:18" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1897,6 +1931,7 @@
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="G9" s="25"/>
       <c r="H9" s="4" t="s">
         <v>2</v>
       </c>
@@ -1924,24 +1959,25 @@
       <c r="Q9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="36" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+      <c r="R9" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="56" x14ac:dyDescent="0.15">
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G10" s="25"/>
       <c r="H10" s="2">
         <v>1</v>
       </c>
@@ -1959,22 +1995,23 @@
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="Q10" s="1"/>
-      <c r="R10" s="21" t="s">
+      <c r="R10" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:18" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:18" ht="56" x14ac:dyDescent="0.15">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="2">
         <v>2</v>
       </c>
@@ -1992,137 +2029,151 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="21"/>
-    </row>
-    <row r="12" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="H12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="N12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="40"/>
-    </row>
-    <row r="13" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-    </row>
-    <row r="14" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="26" t="s">
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="N12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="H14" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="26" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J14" s="25"/>
-    </row>
-    <row r="15" spans="2:18" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J14" s="15"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="G15" s="25"/>
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:18" s="30" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="16" t="s">
+    <row r="16" spans="2:18" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="15" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="G16" s="25"/>
       <c r="H16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="28" t="s">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="H17" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-    </row>
-    <row r="18" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="8" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="H18" s="8" t="s">
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="2:12" s="30" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
         <v>2</v>
       </c>
@@ -2138,6 +2189,7 @@
       <c r="F19" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="G19" s="25"/>
       <c r="H19" s="4" t="s">
         <v>2</v>
       </c>
@@ -2154,206 +2206,227 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:12" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G20" s="25"/>
       <c r="H20" s="2">
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:12" s="30" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2">
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G21" s="25"/>
       <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:12" ht="28" x14ac:dyDescent="0.15">
       <c r="B22" s="2">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G22" s="25"/>
       <c r="H22" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="2:12" s="30" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:12" ht="56" x14ac:dyDescent="0.15">
       <c r="B23" s="2">
         <v>4</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="23"/>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-    </row>
-    <row r="24" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="G23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B24" s="2">
         <v>5</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="23"/>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-    </row>
-    <row r="25" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="G24" s="25"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="23"/>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-    </row>
-    <row r="26" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="G25" s="25"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B26" s="2">
         <v>7</v>
       </c>
-      <c r="C26" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="23"/>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-    </row>
-    <row r="27" spans="2:12" s="30" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="G26" s="25"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B27" s="2">
         <v>8</v>
       </c>
-      <c r="C27" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="23"/>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
-    </row>
-    <row r="28" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B28" s="2"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="1"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-    </row>
-    <row r="29" spans="2:12" s="30" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="H29" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B29" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:L8"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="H18:L18"/>
     <mergeCell ref="B29:F29"/>
@@ -2364,19 +2437,6 @@
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="H17:L17"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="O6:Q6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Largely done week four description.
</commit_message>
<xml_diff>
--- a/final/tests/4.3.1_test_set.xlsx
+++ b/final/tests/4.3.1_test_set.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagefleming/university_of_london/current_courses/agile_software_projects/cm2020/final/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE00689-FC50-EE4D-AB75-9A8B475B266B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA498BD6-D022-9F40-A353-0AC6B4CC9269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.3.1 Jan-19th" sheetId="1" r:id="rId1"/>
-    <sheet name="4.3.1 (EMPTY)" sheetId="9" r:id="rId2"/>
+    <sheet name="4.3.1 (Feb 2nd)" sheetId="10" r:id="rId2"/>
+    <sheet name="4.3.1 (EMPTY)" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="79">
   <si>
     <t>Objective and Priority</t>
   </si>
@@ -260,6 +261,12 @@
   </si>
   <si>
     <t>Continue to test 4.3.1.2.3.2</t>
+  </si>
+  <si>
+    <t>youtube.com is blocked.</t>
+  </si>
+  <si>
+    <t>Url is unaccessible.</t>
   </si>
 </sst>
 </file>
@@ -510,6 +517,42 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -517,42 +560,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -943,7 +950,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -977,20 +984,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
@@ -1034,11 +1041,11 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1046,11 +1053,11 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1071,11 +1078,11 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1083,67 +1090,67 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="39" t="s">
+      <c r="N7" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="41"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="33"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
       <c r="M8" s="25"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
@@ -1281,21 +1288,21 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
       <c r="N12" s="20" t="s">
         <v>75</v>
       </c>
@@ -1336,11 +1343,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1348,11 +1355,11 @@
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1361,11 +1368,11 @@
       <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1373,48 +1380,48 @@
       <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
     </row>
     <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
@@ -1656,23 +1663,34 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="H29" s="35" t="s">
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="H29" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H29:L29"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="I15:K15"/>
@@ -1685,17 +1703,6 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="H7:L7"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1707,6 +1714,773 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7742FCAD-D72E-CF4F-9C26-A80E845A9012}">
+  <dimension ref="B1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="16"/>
+    <col min="8" max="8" width="29" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="16"/>
+    <col min="14" max="14" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="16" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="16" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="16"/>
+    <col min="20" max="20" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" style="16" customWidth="1"/>
+    <col min="22" max="22" width="28.6640625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.6640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B1" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="28" x14ac:dyDescent="0.15">
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B7" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="33"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B8" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="N9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="56" x14ac:dyDescent="0.15">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="56" x14ac:dyDescent="0.15">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="25"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B12" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="N12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+    </row>
+    <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="25"/>
+      <c r="H19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="2:12" ht="28" x14ac:dyDescent="0.15">
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="2:12" ht="56" x14ac:dyDescent="0.15">
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B26" s="2">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B27" s="2">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B28" s="2"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B29" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="H29" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="O6:Q6"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F4918A-11B6-0341-821A-120D4920BA32}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:R29"/>
@@ -1745,20 +2519,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
@@ -1799,11 +2573,11 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1811,11 +2585,11 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1835,11 +2609,11 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1847,66 +2621,66 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="36" t="s">
+      <c r="O6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="38"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="N7" s="39" t="s">
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="N7" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="41"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="33"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="33" t="s">
+      <c r="H8" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
       </c>
@@ -2032,21 +2806,21 @@
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
       <c r="N12" s="20" t="s">
         <v>75</v>
       </c>
@@ -2093,11 +2867,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2105,11 +2879,11 @@
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2118,11 +2892,11 @@
       <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2130,48 +2904,48 @@
       <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
     </row>
     <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
@@ -2397,23 +3171,33 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="H29" s="35" t="s">
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="H29" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:L17"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="H12:L12"/>
@@ -2427,16 +3211,6 @@
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="H8:L8"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:L17"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
WOrk on tests sets and weeks 6-7
</commit_message>
<xml_diff>
--- a/final/tests/4.3.1_test_set.xlsx
+++ b/final/tests/4.3.1_test_set.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gagefleming/university_of_london/current_courses/agile_software_projects/cm2020/final/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA498BD6-D022-9F40-A353-0AC6B4CC9269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E25FCB-ECF4-AA44-87A4-23E5CC65DC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.3.1 Jan-19th" sheetId="1" r:id="rId1"/>
     <sheet name="4.3.1 (Feb 2nd)" sheetId="10" r:id="rId2"/>
-    <sheet name="4.3.1 (EMPTY)" sheetId="9" r:id="rId3"/>
+    <sheet name="4.3.1 (Mar 2nd)" sheetId="11" r:id="rId3"/>
+    <sheet name="4.3.1 (EMPTY)" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="82">
   <si>
     <t>Objective and Priority</t>
   </si>
@@ -267,6 +268,15 @@
   </si>
   <si>
     <t>Url is unaccessible.</t>
+  </si>
+  <si>
+    <t>Displays last active course..</t>
+  </si>
+  <si>
+    <t>Correctly updates</t>
+  </si>
+  <si>
+    <t>Data dashboard button works as intended.</t>
   </si>
 </sst>
 </file>
@@ -517,6 +527,30 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -535,31 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -651,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -691,7 +701,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -797,7 +807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -939,7 +949,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -984,20 +994,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
@@ -1041,11 +1051,11 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1053,11 +1063,11 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1078,11 +1088,11 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1090,67 +1100,67 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
       <c r="M8" s="25"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
@@ -1288,21 +1298,21 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
       <c r="N12" s="20" t="s">
         <v>75</v>
       </c>
@@ -1343,11 +1353,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1355,11 +1365,11 @@
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1368,11 +1378,11 @@
       <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1380,48 +1390,48 @@
       <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
@@ -1663,34 +1673,23 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="H29" s="39" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="H29:L29"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="I15:K15"/>
@@ -1703,6 +1702,17 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="H7:L7"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1717,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7742FCAD-D72E-CF4F-9C26-A80E845A9012}">
   <dimension ref="B1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1751,20 +1761,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
@@ -1808,11 +1818,11 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1820,11 +1830,11 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1845,11 +1855,11 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1857,67 +1867,67 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="25"/>
-      <c r="N7" s="31" t="s">
+      <c r="N7" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
       <c r="M8" s="25"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
@@ -2055,21 +2065,21 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
       <c r="N12" s="20" t="s">
         <v>75</v>
       </c>
@@ -2110,11 +2120,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2122,11 +2132,11 @@
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2135,11 +2145,11 @@
       <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2147,48 +2157,48 @@
       <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
@@ -2430,20 +2440,789 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="H29" s="39" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:L17"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7AA0F5E-6032-4C43-84FD-99882B016D22}">
+  <dimension ref="B1:R29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="16"/>
+    <col min="8" max="8" width="29" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="16"/>
+    <col min="14" max="14" width="26" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="16" customWidth="1"/>
+    <col min="16" max="16" width="20.5" style="16" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="16"/>
+    <col min="20" max="20" width="16.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" style="16" customWidth="1"/>
+    <col min="22" max="22" width="28.6640625" style="16" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="11.6640625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B1" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="N5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="28" x14ac:dyDescent="0.15">
+      <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B7" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B8" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:18" ht="14" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="N9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="56" x14ac:dyDescent="0.15">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="N10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="56" x14ac:dyDescent="0.15">
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="25"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B12" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="N12" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="22"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="15"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.15">
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="32" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B17" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+    </row>
+    <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="25"/>
+      <c r="H19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="2:12" ht="28" x14ac:dyDescent="0.15">
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="25"/>
+      <c r="H22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="2:12" ht="56" x14ac:dyDescent="0.15">
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B26" s="2">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="2:12" ht="42" x14ac:dyDescent="0.15">
+      <c r="B27" s="2">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B28" s="2"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="1"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B29" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -2480,7 +3259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F4918A-11B6-0341-821A-120D4920BA32}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:R29"/>
@@ -2519,20 +3298,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B3" s="17"/>
@@ -2573,11 +3352,11 @@
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2585,11 +3364,11 @@
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
       <c r="L5" s="3" t="s">
         <v>16</v>
       </c>
@@ -2609,11 +3388,11 @@
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2621,66 +3400,66 @@
       <c r="H6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="38"/>
       <c r="R6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="N7" s="31" t="s">
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="N7" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
       <c r="N8" s="5" t="s">
         <v>1</v>
       </c>
@@ -2806,21 +3585,21 @@
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="25"/>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
       <c r="N12" s="20" t="s">
         <v>75</v>
       </c>
@@ -2867,11 +3646,11 @@
       <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
       <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2879,11 +3658,11 @@
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
       <c r="L15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2892,11 +3671,11 @@
       <c r="B16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="8" t="s">
         <v>8</v>
       </c>
@@ -2904,48 +3683,48 @@
       <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="25"/>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="2:12" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="4" t="s">
@@ -3171,33 +3950,23 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="H29" s="39" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="H29" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:L17"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="H12:L12"/>
@@ -3211,6 +3980,16 @@
     <mergeCell ref="N7:R7"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="H8:L8"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:L17"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>